<commit_message>
add iziToast, add again moment js dan daterangepicker
</commit_message>
<xml_diff>
--- a/hasil/2023_01_lipa_18.xlsx
+++ b/hasil/2023_01_lipa_18.xlsx
@@ -239,7 +239,7 @@
     <t>Mengetahui</t>
   </si>
   <si>
-    <t>Ternate , 17 Juli 2023</t>
+    <t>Ternate , 02 Agustus 2023</t>
   </si>
   <si>
     <t>Ketua Pengadilan Agama Ternate ,</t>
@@ -267,7 +267,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -321,6 +321,15 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Narrow"/>
     </font>
   </fonts>
   <fills count="6">
@@ -522,11 +531,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
-    <xf xfId="0" fontId="4" numFmtId="164" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+    <xf xfId="0" fontId="6" numFmtId="164" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>

</xml_diff>

<commit_message>
add view table laporan lipa 18
</commit_message>
<xml_diff>
--- a/hasil/2023_01_lipa_18.xlsx
+++ b/hasil/2023_01_lipa_18.xlsx
@@ -239,7 +239,7 @@
     <t>Mengetahui</t>
   </si>
   <si>
-    <t>Ternate , 02 Agustus 2023</t>
+    <t>Ternate , 06 September 2023</t>
   </si>
   <si>
     <t>Ketua Pengadilan Agama Ternate ,</t>
@@ -1310,7 +1310,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="30">
-        <v>0</v>
+        <v>163500</v>
       </c>
       <c r="C15" s="30">
         <v>590000</v>
@@ -1334,10 +1334,10 @@
         <v>0</v>
       </c>
       <c r="J15" s="30">
-        <v>0</v>
+        <v>670000</v>
       </c>
       <c r="K15" s="30">
-        <v>0</v>
+        <v>690000</v>
       </c>
       <c r="L15" s="30">
         <v>0</v>
@@ -1349,7 +1349,7 @@
         <v>0</v>
       </c>
       <c r="O15" s="30">
-        <v>0</v>
+        <v>340000</v>
       </c>
       <c r="P15" s="30">
         <v>0</v>
@@ -1358,7 +1358,7 @@
         <v>0</v>
       </c>
       <c r="R15" s="30">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="S15" s="30" t="str">
         <f>sum(B15:R15)</f>

</xml_diff>